<commit_message>
#38 Finished GetCategories with hierarchy
</commit_message>
<xml_diff>
--- a/cintamani-next/data/products/products_test.xlsx
+++ b/cintamani-next/data/products/products_test.xlsx
@@ -438,7 +438,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A4" sqref="A4:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,13 +522,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4">
         <v>250</v>
@@ -545,13 +545,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5">
         <v>250</v>
@@ -568,13 +568,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D6">
         <v>250</v>
@@ -591,13 +591,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D7">
         <v>250</v>

</xml_diff>